<commit_message>
Added Alex as VPPE
</commit_message>
<xml_diff>
--- a/src/data/current_data/leadership_currentdata.xlsx
+++ b/src/data/current_data/leadership_currentdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicalin/dsp_vs_code/dspuci-website-gatsby/src/data/current_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C20FB2-D521-4B43-A051-1609D4809319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07620B68-005C-F94A-A19D-B5876DC0492C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15840" xr2:uid="{2C0ED811-1999-2046-A233-A574ADF233C5}"/>
   </bookViews>
@@ -96,7 +96,7 @@
     <t>Juliana Lee</t>
   </si>
   <si>
-    <t>tba</t>
+    <t>Alex Pham</t>
   </si>
 </sst>
 </file>
@@ -466,7 +466,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated directors and ec
</commit_message>
<xml_diff>
--- a/src/data/current_data/leadership_currentdata.xlsx
+++ b/src/data/current_data/leadership_currentdata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -40,40 +40,43 @@
     <t>Vice President of Pledge Education</t>
   </si>
   <si>
-    <t>Jacob Lee</t>
+    <t>Tommy Wunsch</t>
   </si>
   <si>
     <t>Vice President of Finance</t>
   </si>
   <si>
-    <t>Ishan Malik</t>
+    <t>Elaine Nguyen</t>
   </si>
   <si>
     <t>Vice President of Chapter Operations</t>
   </si>
   <si>
-    <t>Jason Henkel</t>
+    <t>Brennan Kim</t>
   </si>
   <si>
     <t>Chancellor</t>
   </si>
   <si>
-    <t>Nithin Senthil</t>
+    <t>Lohit Potnuru</t>
   </si>
   <si>
     <t>Vice President of Professional Activities</t>
   </si>
   <si>
-    <t>Juliana Lee</t>
+    <t>Jessica Lin</t>
   </si>
   <si>
     <t>Vice President of Community Service</t>
   </si>
   <si>
+    <t>Melanie Sagun</t>
+  </si>
+  <si>
     <t>Vice President of Scholarship and Awards</t>
   </si>
   <si>
-    <t>Diana Huynh</t>
+    <t>Isaac Martinez</t>
   </si>
   <si>
     <t>Vice President of Alumni Relations</t>
@@ -142,7 +145,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -530,18 +533,18 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="2" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>